<commit_message>
feat: Mainscene에 db 추가
</commit_message>
<xml_diff>
--- a/Database/worksheet.xlsx
+++ b/Database/worksheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ykkim\github\doccas\Database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{596803EA-D3D3-4F81-BAEF-8A10F85E7FD9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDEAD778-A3F1-4D15-ACC4-72D97C289204}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -44,10 +44,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>health</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>cleanliness</t>
   </si>
   <si>
@@ -76,16 +72,21 @@
     <t>playTime</t>
   </si>
   <si>
+    <t>lastAccess</t>
+  </si>
+  <si>
+    <t>사용자</t>
+  </si>
+  <si>
+    <t>김누구</t>
+  </si>
+  <si>
+    <t>likability</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>depression</t>
-  </si>
-  <si>
-    <t>lastAccess</t>
-  </si>
-  <si>
-    <t>사용자</t>
-  </si>
-  <si>
-    <t>김누구</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -422,81 +423,72 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="1" width="8.796875" style="1"/>
     <col min="2" max="2" width="10.8984375" style="1" customWidth="1"/>
     <col min="3" max="3" width="8.796875" style="1"/>
-    <col min="4" max="4" width="16.8984375" style="1" customWidth="1"/>
-    <col min="5" max="5" width="13.19921875" style="1" customWidth="1"/>
-    <col min="6" max="16384" width="8.796875" style="1"/>
+    <col min="4" max="4" width="13.19921875" style="1" customWidth="1"/>
+    <col min="5" max="16384" width="8.796875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D1" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="F1" s="2"/>
+      <c r="E1" s="2"/>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A2" s="2">
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C2" s="3">
         <v>0.20833333333333334</v>
       </c>
-      <c r="D2" s="2">
-        <v>40</v>
-      </c>
-      <c r="E2" s="4">
+      <c r="D2" s="4">
         <v>45134</v>
       </c>
-      <c r="F2" s="2"/>
+      <c r="E2" s="2"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A3" s="2">
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C3" s="3">
         <v>0.29236111111111113</v>
       </c>
-      <c r="D3" s="2">
-        <v>41</v>
-      </c>
-      <c r="E3" s="4">
+      <c r="D3" s="4">
         <v>45135</v>
       </c>
-      <c r="F3" s="2"/>
+      <c r="E3" s="2"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A4" s="2"/>
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -506,26 +498,26 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{52DE7A94-CE18-49B8-8098-C9FA167CB6E3}">
-  <dimension ref="A1:J2"/>
+  <dimension ref="A1:K2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="L6" sqref="L6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="1" width="8.796875" style="1"/>
     <col min="2" max="3" width="10.8984375" style="1" customWidth="1"/>
-    <col min="4" max="5" width="8.796875" style="1"/>
-    <col min="6" max="6" width="10.69921875" style="1" customWidth="1"/>
-    <col min="7" max="9" width="8.796875" style="1"/>
-    <col min="10" max="10" width="11.59765625" style="1" customWidth="1"/>
-    <col min="11" max="16384" width="8.796875" style="1"/>
+    <col min="4" max="4" width="8.796875" style="1"/>
+    <col min="5" max="6" width="10.69921875" style="1" customWidth="1"/>
+    <col min="7" max="10" width="8.796875" style="1"/>
+    <col min="11" max="11" width="11.59765625" style="1" customWidth="1"/>
+    <col min="12" max="16384" width="8.796875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A1" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -534,28 +526,31 @@
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>5</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>6</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
       <c r="I1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="K1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
-        <v>9</v>
-      </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -566,24 +561,27 @@
         <v>1</v>
       </c>
       <c r="D2" s="1">
-        <v>12000</v>
+        <v>88</v>
       </c>
       <c r="E2" s="1">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="F2" s="1">
-        <v>85</v>
+        <v>60</v>
       </c>
       <c r="G2" s="1">
         <v>70</v>
       </c>
       <c r="H2" s="1">
+        <v>3</v>
+      </c>
+      <c r="I2" s="1">
+        <v>12000</v>
+      </c>
+      <c r="J2" s="1">
         <v>525</v>
       </c>
-      <c r="I2" s="1">
-        <v>3</v>
-      </c>
-      <c r="J2" s="1">
+      <c r="K2" s="1">
         <v>12</v>
       </c>
     </row>

</xml_diff>